<commit_message>
Added functionality for weapon swapping Added Machine Pistol
</commit_message>
<xml_diff>
--- a/Weapons.xlsx
+++ b/Weapons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Project Blam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CBC72D-D8A8-4119-9781-70B97FE8F767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3FE88E-735E-4AC3-8213-2C38102FB8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{22FDCC58-3935-4D06-95CE-1A0D1701BC1B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="95">
   <si>
     <t>Weapon</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Health%</t>
   </si>
   <si>
-    <t>Walk%</t>
-  </si>
-  <si>
     <t>Clip</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Rounds</t>
-  </si>
-  <si>
-    <t>Per Burst</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>Accel End</t>
   </si>
   <si>
-    <t>8%</t>
-  </si>
-  <si>
     <t>12%</t>
   </si>
   <si>
@@ -234,9 +222,6 @@
     <t>Bounce Combo</t>
   </si>
   <si>
-    <t>Auto</t>
-  </si>
-  <si>
     <t>5%</t>
   </si>
   <si>
@@ -282,9 +267,6 @@
     <t>Conical Spread</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>1%</t>
   </si>
   <si>
@@ -306,15 +288,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>1 set of 9</t>
-  </si>
-  <si>
-    <t>1 set of 15</t>
-  </si>
-  <si>
-    <t>1 set of 5</t>
-  </si>
-  <si>
     <t>Spread Zoning</t>
   </si>
   <si>
@@ -325,6 +298,24 @@
   </si>
   <si>
     <t>Raygun</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Unit%</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Bullets</t>
+  </si>
+  <si>
+    <t>Per Shot</t>
   </si>
 </sst>
 </file>
@@ -686,7 +677,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +694,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -712,31 +703,31 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>5</v>
@@ -744,47 +735,47 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -796,112 +787,112 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>91</v>
@@ -910,60 +901,60 @@
         <v>8</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="1" t="s">
@@ -973,226 +964,226 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>92</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B12" s="3"/>
       <c r="O12" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1207,32 +1198,35 @@
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
@@ -1243,9 +1237,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>